<commit_message>
hw5: plot kmeans for elec, therm data
this is normalized data though. next step: plot the non-normalized data, and add titles to plots n all
</commit_message>
<xml_diff>
--- a/hw/hw5/Steel_data_for_clustering.xlsx
+++ b/hw/hw5/Steel_data_for_clustering.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\seanp\Downloads\21F_MECH_ENG_395\hw\hw5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8692A5E-6081-4F96-8EE4-774EBCC99E83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF96D767-B593-4DC7-924D-66332E206754}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Steel_data_for_clustering" sheetId="1" r:id="rId1"/>
@@ -1038,7 +1038,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="J18" sqref="J18"/>
     </sheetView>
@@ -2499,8 +2499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2753A2E-DFC8-411E-A594-E5430B2B7706}">
   <dimension ref="A1:M41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2509,7 +2509,10 @@
     <col min="2" max="2" width="11.77734375" customWidth="1"/>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
     <col min="4" max="7" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="12" width="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.109375" customWidth="1"/>
+    <col min="11" max="11" width="19.77734375" customWidth="1"/>
+    <col min="12" max="12" width="31.109375" customWidth="1"/>
     <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>